<commit_message>
Work an Alt by Bo
</commit_message>
<xml_diff>
--- a/CH-165 Customer Grouping.xlsx
+++ b/CH-165 Customer Grouping.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2176E603-8A7A-42D8-8072-48FFFE2E142E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66000D20-BE2C-42AA-ADFC-85E5CC4C2BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$3:$B$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$3:$B$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
   <si>
     <t>Result</t>
   </si>
@@ -980,12 +1004,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="9">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7D8E6F56-5B41-46CE-9ED7-4E67C0ACC856}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1267,4 +1318,410 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB67C699-43F0-48F1-B81F-1E2D3C2DB0EB}">
+  <dimension ref="B1:M18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.8984375" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3984375" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.19921875" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.59765625" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="F1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="L1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="15">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="20">
+        <v>2</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="23"/>
+    </row>
+    <row r="4" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="15">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="20">
+        <v>3</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="15">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="20">
+        <v>4</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="15">
+        <v>27</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="24">
+        <v>5</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="27"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13">
+        <v>3</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="15">
+        <v>36</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="13">
+        <v>3</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="15">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="13">
+        <v>3</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="15">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="13">
+        <v>4</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15">
+        <v>34</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="18">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D12" s="11"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="str" cm="1">
+        <f t="array" ref="B14:F18">_xlfn.LET(
+    _xlpm.m, B3:B11,
+    _xlpm.c, C3:C11,
+    _xlpm.n, _xlfn.XLOOKUP(_xlpm.c, _xlpm.c, _xlpm.m) = _xlpm.m,
+    _xlpm.y, ISNA(_xlfn.XMATCH(_xlpm.c &amp; _xlpm.m - 1, _xlpm.c &amp; _xlpm.m)),
+    _xlfn.VSTACK(
+        {"Month","New","ACTIVE","Inactive","Returning"},
+        _xlfn.DROP(
+            _xlfn.GROUPBY(
+                _xlpm.m,
+                _xlfn.HSTACK(
+                    REPT(_xlpm.c, _xlpm.n),
+                    REPT(_xlpm.c, 1 - _xlpm.y),
+                    _xlfn.MAP(
+                        _xlpm.m,
+                        _xlfn.LAMBDA(_xlpm.i,
+                            _xlfn.ARRAYTOTEXT(
+                                _xlfn.UNIQUE(
+                                    _xlfn._xlws.FILTER(
+                                        _xlpm.c,
+                                        (_xlpm.m &lt; _xlpm.i) * ISNA(_xlfn.XMATCH(_xlpm.c, _xlfn._xlws.FILTER(_xlpm.c, _xlpm.m = _xlpm.i))),
+                                        ""
+                                    )
+                                )
+                            )
+                        )
+                    ),
+                    REPT(_xlpm.c, _xlpm.y * (1 - _xlpm.n))
+                ),
+                _xlfn.LAMBDA(_xlpm.x, _xlfn.TEXTJOIN(", ", , _xlfn.UNIQUE(_xlpm.x))),
+                ,
+                0
+            ),
+            1
+        )
+    )
+)</f>
+        <v>Month</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <v>New</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <v>ACTIVE</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Inactive</v>
+      </c>
+      <c r="F14" s="30" t="str">
+        <v>Returning</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <v>C</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <v>A</v>
+      </c>
+      <c r="E15" t="str">
+        <v>B</v>
+      </c>
+      <c r="F15" s="30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <v/>
+      </c>
+      <c r="D16" s="2" t="str">
+        <v>A, C</v>
+      </c>
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" s="30" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <v/>
+      </c>
+      <c r="D17" s="2" t="str">
+        <v>A</v>
+      </c>
+      <c r="E17" t="str">
+        <v>B, C</v>
+      </c>
+      <c r="F17" s="30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <v>D</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E18" t="str">
+        <v>A, B, C</v>
+      </c>
+      <c r="F18" s="30" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I have broken Bo's solution down.
</commit_message>
<xml_diff>
--- a/CH-165 Customer Grouping.xlsx
+++ b/CH-165 Customer Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66000D20-BE2C-42AA-ADFC-85E5CC4C2BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD63B92-8499-4BE3-B513-88F80A257B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,17 @@
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_c">'Alt1'!$C$3:$C$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$3:$B$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$3:$B$11</definedName>
+    <definedName name="_m">'Alt1'!$B$3:$B$11</definedName>
+    <definedName name="_n">'Alt1'!$B$22:$B$30</definedName>
+    <definedName name="_y">'Alt1'!$C$22:$C$30</definedName>
+    <definedName name="_z">'Alt1'!$D$22:$G$30</definedName>
+    <definedName name="_z1">'Alt1'!$D$22:$D$30</definedName>
+    <definedName name="_z2">'Alt1'!$E$22:$E$30</definedName>
+    <definedName name="_z3">'Alt1'!$F$22:$F$30</definedName>
+    <definedName name="_ZZ">'Alt1'!$G$22:$G$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>Result</t>
   </si>
@@ -114,6 +123,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
+  </si>
+  <si>
+    <t>Inactiv</t>
   </si>
 </sst>
 </file>
@@ -375,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -461,6 +473,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1322,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB67C699-43F0-48F1-B81F-1E2D3C2DB0EB}">
-  <dimension ref="B1:M18"/>
+  <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1682,7 +1697,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>4</v>
       </c>
@@ -1699,7 +1714,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>5</v>
       </c>
@@ -1713,6 +1728,331 @@
         <v>A, B, C</v>
       </c>
       <c r="F18" s="30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="b" cm="1">
+        <f t="array" ref="B22:B30">_xlfn.XLOOKUP(_c, _c, _m) = _m</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="b" cm="1">
+        <f t="array" ref="C22:C30">ISNA(_xlfn.XMATCH(_c &amp; _m - 1, _c &amp; _m))</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="str" cm="1">
+        <f t="array" ref="D22:D30">REPT(_c, _n)</f>
+        <v>A</v>
+      </c>
+      <c r="E22" s="30" t="str" cm="1">
+        <f t="array" ref="E22:E30">REPT(_c, 1 - _y)</f>
+        <v/>
+      </c>
+      <c r="F22" t="str" cm="1">
+        <f t="array" ref="F22:F30" xml:space="preserve">                    _xlfn.MAP(
+                        _m,
+                        _xlfn.LAMBDA(_xlpm.i,
+                            _xlfn.ARRAYTOTEXT(
+                                _xlfn.UNIQUE(
+                                    _xlfn._xlws.FILTER(
+                                        _c,
+                                        (_m &lt; _xlpm.i) * ISNA(_xlfn.XMATCH(_c, _xlfn._xlws.FILTER(_c, _m = _xlpm.i))),
+                                        ""
+                                    )
+                                )
+                            )
+                        )
+                    )</f>
+        <v/>
+      </c>
+      <c r="G22" s="30" t="str" cm="1">
+        <f t="array" ref="G22:G30">REPT(_c, _y * (1 - _n))</f>
+        <v/>
+      </c>
+      <c r="H22" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <v>B</v>
+      </c>
+      <c r="E23" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+      <c r="G23" s="30" t="str">
+        <v/>
+      </c>
+      <c r="H23" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E24" s="30" t="str">
+        <v>A</v>
+      </c>
+      <c r="F24" t="str">
+        <v>B</v>
+      </c>
+      <c r="G24" s="30" t="str">
+        <v/>
+      </c>
+      <c r="H24" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <v>C</v>
+      </c>
+      <c r="E25" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F25" t="str">
+        <v>B</v>
+      </c>
+      <c r="G25" s="30" t="str">
+        <v/>
+      </c>
+      <c r="H25" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E26" s="30" t="str">
+        <v>A</v>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+      <c r="G26" s="30" t="str">
+        <v/>
+      </c>
+      <c r="H26" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E27" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F27" t="str">
+        <v/>
+      </c>
+      <c r="G27" s="30" t="str">
+        <v>B</v>
+      </c>
+      <c r="H27" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E28" s="30" t="str">
+        <v>C</v>
+      </c>
+      <c r="F28" t="str">
+        <v/>
+      </c>
+      <c r="G28" s="30" t="str">
+        <v/>
+      </c>
+      <c r="H28" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E29" s="30" t="str">
+        <v>A</v>
+      </c>
+      <c r="F29" t="str">
+        <v>B, C</v>
+      </c>
+      <c r="G29" s="30" t="str">
+        <v/>
+      </c>
+      <c r="H29" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="str">
+        <v>D</v>
+      </c>
+      <c r="E30" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F30" t="str">
+        <v>A, B, C</v>
+      </c>
+      <c r="G30" s="30" t="str">
+        <v/>
+      </c>
+      <c r="H30" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="32" cm="1">
+        <f t="array" ref="B33:F37">_xlfn.GROUPBY(
+                _m,
+                _z,
+                _xlfn.LAMBDA(_xlpm.x, _xlfn.TEXTJOIN(", ", , _xlfn.UNIQUE(_xlpm.x))),,0
+            )</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="str">
+        <v>A, B</v>
+      </c>
+      <c r="D33" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E33" t="str">
+        <v/>
+      </c>
+      <c r="F33" s="30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <v>C</v>
+      </c>
+      <c r="D34" s="2" t="str">
+        <v>A</v>
+      </c>
+      <c r="E34" t="str">
+        <v>B</v>
+      </c>
+      <c r="F34" s="30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2" t="str">
+        <v/>
+      </c>
+      <c r="D35" s="2" t="str">
+        <v>A, C</v>
+      </c>
+      <c r="E35" t="str">
+        <v/>
+      </c>
+      <c r="F35" s="30" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2" t="str">
+        <v/>
+      </c>
+      <c r="D36" s="2" t="str">
+        <v>A</v>
+      </c>
+      <c r="E36" t="str">
+        <v>B, C</v>
+      </c>
+      <c r="F36" s="30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>5</v>
+      </c>
+      <c r="C37" s="2" t="str">
+        <v>D</v>
+      </c>
+      <c r="D37" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E37" t="str">
+        <v>A, B, C</v>
+      </c>
+      <c r="F37" s="30" t="str">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
I now understand how to find the first item when there are a bunch of repeats.
</commit_message>
<xml_diff>
--- a/CH-165 Customer Grouping.xlsx
+++ b/CH-165 Customer Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD63B92-8499-4BE3-B513-88F80A257B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57DDD4D-1895-423B-82E9-71C411D595E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="26">
   <si>
     <t>Result</t>
   </si>
@@ -126,6 +126,30 @@
   </si>
   <si>
     <t>Inactiv</t>
+  </si>
+  <si>
+    <t>I need to understand how the new items are found.</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Pat</t>
+  </si>
+  <si>
+    <t>Katee</t>
+  </si>
+  <si>
+    <t>It is yet another way to perform a filter operation.</t>
+  </si>
+  <si>
+    <t>Find the first item.</t>
   </si>
 </sst>
 </file>
@@ -471,11 +495,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1037,6 +1061,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1071,18 +1098,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="F1" s="31" t="s">
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="F1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1337,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB67C699-43F0-48F1-B81F-1E2D3C2DB0EB}">
-  <dimension ref="B1:M37"/>
+  <dimension ref="B1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1360,18 +1387,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="F1" s="31" t="s">
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="F1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1697,7 +1724,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>4</v>
       </c>
@@ -1714,7 +1741,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>5</v>
       </c>
@@ -1731,7 +1758,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1740,7 +1767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="b" cm="1">
         <f t="array" ref="B22:B30">_xlfn.XLOOKUP(_c, _c, _m) = _m</f>
         <v>1</v>
@@ -1782,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="b">
         <v>1</v>
       </c>
@@ -1805,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="b">
         <v>0</v>
       </c>
@@ -1828,7 +1855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="b">
         <v>1</v>
       </c>
@@ -1851,7 +1878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="b">
         <v>0</v>
       </c>
@@ -1874,7 +1901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="b">
         <v>0</v>
       </c>
@@ -1897,7 +1924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="b">
         <v>0</v>
       </c>
@@ -1920,7 +1947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="b">
         <v>0</v>
       </c>
@@ -1943,7 +1970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="b">
         <v>1</v>
       </c>
@@ -1966,8 +1993,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="32" cm="1">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="31" cm="1">
         <f t="array" ref="B33:F37">_xlfn.GROUPBY(
                 _m,
                 _z,
@@ -1987,8 +2019,11 @@
       <c r="F33" s="30" t="str">
         <v/>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>2</v>
       </c>
@@ -2004,8 +2039,18 @@
       <c r="F34" s="30" t="str">
         <v/>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34" t="str" cm="1">
+        <f t="array" ref="M34:M38">REPT(K34:K38,L34:L38)</f>
+        <v>Mark</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>3</v>
       </c>
@@ -2021,8 +2066,17 @@
       <c r="F35" s="30" t="str">
         <v>B</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>4</v>
       </c>
@@ -2038,8 +2092,17 @@
       <c r="F36" s="30" t="str">
         <v/>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36" t="str">
+        <v>Tim</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>5</v>
       </c>
@@ -2054,6 +2117,142 @@
       </c>
       <c r="F37" s="30" t="str">
         <v/>
+      </c>
+      <c r="K37" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>23</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38" t="str">
+        <v>Katee</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="N44" t="b" cm="1">
+        <f t="array" ref="N44:N53">_xlfn.XLOOKUP(K44:K53,K44:K53,L44:L53)=L44:L53</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45">
+        <v>2</v>
+      </c>
+      <c r="N45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>19</v>
+      </c>
+      <c r="L46">
+        <v>3</v>
+      </c>
+      <c r="N46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L47">
+        <v>4</v>
+      </c>
+      <c r="N47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>21</v>
+      </c>
+      <c r="L48">
+        <v>5</v>
+      </c>
+      <c r="N48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>22</v>
+      </c>
+      <c r="L49">
+        <v>6</v>
+      </c>
+      <c r="N49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>22</v>
+      </c>
+      <c r="L50">
+        <v>7</v>
+      </c>
+      <c r="N50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>23</v>
+      </c>
+      <c r="L51">
+        <v>8</v>
+      </c>
+      <c r="N51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
+        <v>23</v>
+      </c>
+      <c r="L52">
+        <v>9</v>
+      </c>
+      <c r="N52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
+        <v>23</v>
+      </c>
+      <c r="L53">
+        <v>10</v>
+      </c>
+      <c r="N53" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I now understand how to determine the active customer
</commit_message>
<xml_diff>
--- a/CH-165 Customer Grouping.xlsx
+++ b/CH-165 Customer Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57DDD4D-1895-423B-82E9-71C411D595E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C43CEC3-6778-44D9-8386-12C39240F00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,11 +18,14 @@
   </sheets>
   <definedNames>
     <definedName name="_c">'Alt1'!$C$3:$C$11</definedName>
+    <definedName name="_CC">'Alt1'!$B$44:$B$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$3:$B$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$3:$B$11</definedName>
     <definedName name="_m">'Alt1'!$B$3:$B$11</definedName>
+    <definedName name="_mm">'Alt1'!$C$44:$C$50</definedName>
     <definedName name="_n">'Alt1'!$B$22:$B$30</definedName>
     <definedName name="_y">'Alt1'!$C$22:$C$30</definedName>
+    <definedName name="_yy">'Alt1'!$D$44:$D$50</definedName>
     <definedName name="_z">'Alt1'!$D$22:$G$30</definedName>
     <definedName name="_z1">'Alt1'!$D$22:$D$30</definedName>
     <definedName name="_z2">'Alt1'!$E$22:$E$30</definedName>
@@ -72,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="27">
   <si>
     <t>Result</t>
   </si>
@@ -150,6 +153,9 @@
   </si>
   <si>
     <t>Find the first item.</t>
+  </si>
+  <si>
+    <t>Collect items that are active in a month</t>
   </si>
 </sst>
 </file>
@@ -196,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +221,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -411,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -500,6 +518,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB67C699-43F0-48F1-B81F-1E2D3C2DB0EB}">
-  <dimension ref="B1:N53"/>
+  <dimension ref="B1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1724,7 +1754,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>4</v>
       </c>
@@ -1741,7 +1771,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>5</v>
       </c>
@@ -1758,7 +1788,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1767,7 +1797,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="b" cm="1">
         <f t="array" ref="B22:B30">_xlfn.XLOOKUP(_c, _c, _m) = _m</f>
         <v>1</v>
@@ -1809,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="b">
         <v>1</v>
       </c>
@@ -1832,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="b">
         <v>0</v>
       </c>
@@ -1855,7 +1885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="b">
         <v>1</v>
       </c>
@@ -1878,7 +1908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="b">
         <v>0</v>
       </c>
@@ -1901,7 +1931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="b">
         <v>0</v>
       </c>
@@ -1924,7 +1954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="b">
         <v>0</v>
       </c>
@@ -1947,7 +1977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="b">
         <v>0</v>
       </c>
@@ -1970,7 +2000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="b">
         <v>1</v>
       </c>
@@ -1993,12 +2023,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K31" t="s">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K31" s="34" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="33"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="33"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="31" cm="1">
         <f t="array" ref="B33:F37">_xlfn.GROUPBY(
                 _m,
@@ -2019,11 +2066,18 @@
       <c r="F33" s="30" t="str">
         <v/>
       </c>
-      <c r="M33" t="s">
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="33"/>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="33"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>2</v>
       </c>
@@ -2039,18 +2093,23 @@
       <c r="F34" s="30" t="str">
         <v/>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-      <c r="M34" t="str" cm="1">
+      <c r="L34" s="33">
+        <v>1</v>
+      </c>
+      <c r="M34" s="33" t="str" cm="1">
         <f t="array" ref="M34:M38">REPT(K34:K38,L34:L38)</f>
         <v>Mark</v>
       </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N34" s="33"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="33"/>
+      <c r="Q34" s="33"/>
+      <c r="R34" s="33"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>3</v>
       </c>
@@ -2066,17 +2125,22 @@
       <c r="F35" s="30" t="str">
         <v>B</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K35" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="33">
         <v>0</v>
       </c>
-      <c r="M35" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M35" s="33" t="str">
+        <v/>
+      </c>
+      <c r="N35" s="33"/>
+      <c r="O35" s="33"/>
+      <c r="P35" s="33"/>
+      <c r="Q35" s="33"/>
+      <c r="R35" s="33"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>4</v>
       </c>
@@ -2092,17 +2156,22 @@
       <c r="F36" s="30" t="str">
         <v/>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="L36">
-        <v>1</v>
-      </c>
-      <c r="M36" t="str">
+      <c r="L36" s="33">
+        <v>1</v>
+      </c>
+      <c r="M36" s="33" t="str">
         <v>Tim</v>
       </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="33"/>
+      <c r="Q36" s="33"/>
+      <c r="R36" s="33"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>5</v>
       </c>
@@ -2118,142 +2187,356 @@
       <c r="F37" s="30" t="str">
         <v/>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="33">
         <v>0</v>
       </c>
-      <c r="M37" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K38" t="s">
+      <c r="M37" s="33" t="str">
+        <v/>
+      </c>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="33"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K38" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="L38">
-        <v>1</v>
-      </c>
-      <c r="M38" t="str">
+      <c r="L38" s="33">
+        <v>1</v>
+      </c>
+      <c r="M38" s="33" t="str">
         <v>Katee</v>
       </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K42" t="s">
+      <c r="N38" s="33"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="33"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="33"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B40" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="37"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="33"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B41" s="36"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="36" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C22)</f>
+        <v>=ISNA(XMATCH(_c &amp; _m - 1, _c &amp; _m))</v>
+      </c>
+      <c r="E41" s="37"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="37"/>
+      <c r="K42" s="33" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K44" t="s">
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="33"/>
+      <c r="Q42" s="33"/>
+      <c r="R42" s="33"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="37"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="33"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B44" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L44">
-        <v>1</v>
-      </c>
-      <c r="N44" t="b" cm="1">
+      <c r="C44" s="36">
+        <v>1</v>
+      </c>
+      <c r="D44" s="36" t="b" cm="1">
+        <f t="array" ref="D44:D50">ISNA(_xlfn.XMATCH(_CC &amp; _mm - 1, _CC&amp; _mm))</f>
+        <v>1</v>
+      </c>
+      <c r="E44" s="37" t="str" cm="1">
+        <f t="array" ref="E44:E50">REPT(_CC,1-_yy)</f>
+        <v/>
+      </c>
+      <c r="K44" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="33">
+        <v>1</v>
+      </c>
+      <c r="M44" s="33"/>
+      <c r="N44" s="33" t="b" cm="1">
         <f t="array" ref="N44:N53">_xlfn.XLOOKUP(K44:K53,K44:K53,L44:L53)=L44:L53</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K45" t="s">
+      <c r="O44" s="33"/>
+      <c r="P44" s="33"/>
+      <c r="Q44" s="33"/>
+      <c r="R44" s="33"/>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="L45">
+      <c r="C45" s="36">
+        <v>1</v>
+      </c>
+      <c r="D45" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" s="37" t="str">
+        <v/>
+      </c>
+      <c r="K45" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" s="33">
         <v>2</v>
       </c>
-      <c r="N45" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K46" t="s">
+      <c r="M45" s="33"/>
+      <c r="N45" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="O45" s="33"/>
+      <c r="P45" s="33"/>
+      <c r="Q45" s="33"/>
+      <c r="R45" s="33"/>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B46" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L46">
+      <c r="C46" s="36">
+        <v>2</v>
+      </c>
+      <c r="D46" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="37" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="K46" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="L46" s="33">
         <v>3</v>
       </c>
-      <c r="N46" t="b">
+      <c r="M46" s="33"/>
+      <c r="N46" s="33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K47" t="s">
+      <c r="O46" s="33"/>
+      <c r="P46" s="33"/>
+      <c r="Q46" s="33"/>
+      <c r="R46" s="33"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="36">
+        <v>2</v>
+      </c>
+      <c r="D47" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" s="37" t="str">
+        <v/>
+      </c>
+      <c r="K47" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="33">
         <v>4</v>
       </c>
-      <c r="N47" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K48" t="s">
+      <c r="M47" s="33"/>
+      <c r="N47" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="O47" s="33"/>
+      <c r="P47" s="33"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="33"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="36">
+        <v>3</v>
+      </c>
+      <c r="D48" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" s="37" t="str">
+        <v/>
+      </c>
+      <c r="K48" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="33">
         <v>5</v>
       </c>
-      <c r="N48" t="b">
+      <c r="M48" s="33"/>
+      <c r="N48" s="33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K49" t="s">
+      <c r="O48" s="33"/>
+      <c r="P48" s="33"/>
+      <c r="Q48" s="33"/>
+      <c r="R48" s="33"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B49" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="36">
+        <v>4</v>
+      </c>
+      <c r="D49" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" s="37" t="str">
+        <v/>
+      </c>
+      <c r="K49" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="33">
         <v>6</v>
       </c>
-      <c r="N49" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K50" t="s">
+      <c r="M49" s="33"/>
+      <c r="N49" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="O49" s="33"/>
+      <c r="P49" s="33"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="33"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B50" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="36">
+        <v>4</v>
+      </c>
+      <c r="D50" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="37" t="str">
+        <v>Katee</v>
+      </c>
+      <c r="K50" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="33">
         <v>7</v>
       </c>
-      <c r="N50" t="b">
+      <c r="M50" s="33"/>
+      <c r="N50" s="33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K51" t="s">
+      <c r="O50" s="33"/>
+      <c r="P50" s="33"/>
+      <c r="Q50" s="33"/>
+      <c r="R50" s="33"/>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K51" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="33">
         <v>8</v>
       </c>
-      <c r="N51" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K52" t="s">
+      <c r="M51" s="33"/>
+      <c r="N51" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="O51" s="33"/>
+      <c r="P51" s="33"/>
+      <c r="Q51" s="33"/>
+      <c r="R51" s="33"/>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K52" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="L52">
+      <c r="L52" s="33">
         <v>9</v>
       </c>
-      <c r="N52" t="b">
+      <c r="M52" s="33"/>
+      <c r="N52" s="33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K53" t="s">
+      <c r="O52" s="33"/>
+      <c r="P52" s="33"/>
+      <c r="Q52" s="33"/>
+      <c r="R52" s="33"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K53" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="33">
         <v>10</v>
       </c>
-      <c r="N53" t="b">
+      <c r="M53" s="33"/>
+      <c r="N53" s="33" t="b">
         <v>0</v>
       </c>
+      <c r="O53" s="33"/>
+      <c r="P53" s="33"/>
+      <c r="Q53" s="33"/>
+      <c r="R53" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
I now understand how to find returning people
</commit_message>
<xml_diff>
--- a/CH-165 Customer Grouping.xlsx
+++ b/CH-165 Customer Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C43CEC3-6778-44D9-8386-12C39240F00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D47DEC-FAB0-4F83-B138-C46A312B4193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,6 +24,7 @@
     <definedName name="_m">'Alt1'!$B$3:$B$11</definedName>
     <definedName name="_mm">'Alt1'!$C$44:$C$50</definedName>
     <definedName name="_n">'Alt1'!$B$22:$B$30</definedName>
+    <definedName name="_nn">'Alt1'!$B$57:$B$63</definedName>
     <definedName name="_y">'Alt1'!$C$22:$C$30</definedName>
     <definedName name="_yy">'Alt1'!$D$44:$D$50</definedName>
     <definedName name="_z">'Alt1'!$D$22:$G$30</definedName>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
   <si>
     <t>Result</t>
   </si>
@@ -156,6 +157,12 @@
   </si>
   <si>
     <t>Collect items that are active in a month</t>
+  </si>
+  <si>
+    <t>Retruning</t>
+  </si>
+  <si>
+    <t>Returing</t>
   </si>
 </sst>
 </file>
@@ -202,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +240,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -429,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -530,6 +543,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,8 +579,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -577,7 +596,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="25681" y="2166622"/>
-          <a:ext cx="7771484" cy="2252978"/>
+          <a:ext cx="7771484" cy="2618738"/>
           <a:chOff x="4180502" y="1860551"/>
           <a:chExt cx="3719869" cy="1961643"/>
         </a:xfrm>
@@ -1107,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -1394,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB67C699-43F0-48F1-B81F-1E2D3C2DB0EB}">
-  <dimension ref="B1:R53"/>
+  <dimension ref="B1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1407,8 +1426,7 @@
     <col min="3" max="3" width="10.19921875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.3984375" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.19921875" style="30" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.3984375" style="30" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.19921875" style="30" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" style="30" bestFit="1" customWidth="1"/>
@@ -1796,6 +1814,9 @@
       <c r="F21" t="s">
         <v>17</v>
       </c>
+      <c r="G21" s="30" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="b" cm="1">
@@ -2538,6 +2559,74 @@
       <c r="Q53" s="33"/>
       <c r="R53" s="33"/>
     </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B55" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="40"/>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B57" s="40" t="b" cm="1">
+        <f t="array" ref="B57:B63">_xlfn.XLOOKUP(_CC, _CC, _mm) = _mm</f>
+        <v>1</v>
+      </c>
+      <c r="C57" s="40" t="str" cm="1">
+        <f t="array" ref="C57:C63">REPT(_CC, _yy * (1 - _nn))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B58" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="C58" s="40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B59" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59" s="40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B60" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="C60" s="40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B61" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="C61" s="40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B62" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" s="40" t="str">
+        <v>Craig</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B63" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" s="40" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
I now understand the inacive category
</commit_message>
<xml_diff>
--- a/CH-165 Customer Grouping.xlsx
+++ b/CH-165 Customer Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D47DEC-FAB0-4F83-B138-C46A312B4193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A61564F-070E-4EAD-B82B-0C773B54BB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
   <si>
     <t>Result</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>Returing</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Inactive is interesting. The customer must have occurred once before.</t>
+  </si>
+  <si>
+    <t>Changed Inactive to list all customers, even those that have not purchased yet.</t>
   </si>
 </sst>
 </file>
@@ -172,13 +181,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -209,7 +224,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +241,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
@@ -439,27 +460,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -468,8 +490,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -490,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -517,10 +539,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -529,29 +551,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1126,7 +1159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M12"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -1404,7 +1437,7 @@
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:J1"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1413,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB67C699-43F0-48F1-B81F-1E2D3C2DB0EB}">
-  <dimension ref="B1:R63"/>
+  <dimension ref="B1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1810,12 +1843,17 @@
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="30"/>
+      <c r="E21" s="30" t="s">
+        <v>29</v>
+      </c>
       <c r="F21" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>27</v>
+      </c>
+      <c r="J21" s="41" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
@@ -2627,6 +2665,161 @@
         <v/>
       </c>
     </row>
+    <row r="66" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B66" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="44"/>
+      <c r="I66" s="41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B67" s="43"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="44"/>
+    </row>
+    <row r="68" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B68" s="43" t="str" cm="1">
+        <f t="array" ref="B68:F72">_xlfn.LET(
+    _xlpm.m, B3:B11,
+    _xlpm.c, C3:C11,
+    _xlpm.n, _xlfn.XLOOKUP(_xlpm.c, _xlpm.c, _xlpm.m) = _xlpm.m,
+    _xlpm.y, ISNA(_xlfn.XMATCH(_xlpm.c &amp; _xlpm.m - 1, _xlpm.c &amp; _xlpm.m)),
+    _xlfn.VSTACK(
+        {"Month","New","ACTIVE","Inactive","Returning"},
+        _xlfn.DROP(
+            _xlfn.GROUPBY(
+                _xlpm.m,
+                _xlfn.HSTACK(
+                    REPT(_xlpm.c, _xlpm.n),
+                    REPT(_xlpm.c, 1 - _xlpm.y),
+                    _xlfn.MAP(
+                        _xlpm.m,
+                        _xlfn.LAMBDA(_xlpm.i,
+                            _xlfn.ARRAYTOTEXT(
+                                _xlfn.UNIQUE(
+                                    _xlfn._xlws.FILTER(
+                                        _xlpm.c,
+                                        (_xlpm.m &lt;&gt; _xlpm.i) * ISNA(_xlfn.XMATCH(_xlpm.c, _xlfn._xlws.FILTER(_xlpm.c, _xlpm.m = _xlpm.i))),
+                                        ""
+                                    )
+                                )
+                            )
+                        )
+                    ),
+                    REPT(_xlpm.c, _xlpm.y * (1 - _xlpm.n))
+                ),
+                _xlfn.LAMBDA(_xlpm.x, _xlfn.TEXTJOIN(", ", , _xlfn.UNIQUE(_xlpm.x))),
+                ,
+                0
+            ),
+            1
+        )
+    )
+)</f>
+        <v>Month</v>
+      </c>
+      <c r="C68" s="43" t="str">
+        <v>New</v>
+      </c>
+      <c r="D68" s="43" t="str">
+        <v>ACTIVE</v>
+      </c>
+      <c r="E68" s="42" t="str">
+        <v>Inactive</v>
+      </c>
+      <c r="F68" s="44" t="str">
+        <v>Returning</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B69" s="43">
+        <v>2</v>
+      </c>
+      <c r="C69" s="43" t="str">
+        <v>C</v>
+      </c>
+      <c r="D69" s="43" t="str">
+        <v>A</v>
+      </c>
+      <c r="E69" s="42" t="str">
+        <v>B, D</v>
+      </c>
+      <c r="F69" s="44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B70" s="43">
+        <v>3</v>
+      </c>
+      <c r="C70" s="43" t="str">
+        <v/>
+      </c>
+      <c r="D70" s="43" t="str">
+        <v>A, C</v>
+      </c>
+      <c r="E70" s="42" t="str">
+        <v>D</v>
+      </c>
+      <c r="F70" s="44" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B71" s="43">
+        <v>4</v>
+      </c>
+      <c r="C71" s="43" t="str">
+        <v/>
+      </c>
+      <c r="D71" s="43" t="str">
+        <v>A</v>
+      </c>
+      <c r="E71" s="42" t="str">
+        <v>B, C, D</v>
+      </c>
+      <c r="F71" s="44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B72" s="43">
+        <v>5</v>
+      </c>
+      <c r="C72" s="43" t="str">
+        <v>D</v>
+      </c>
+      <c r="D72" s="43" t="str">
+        <v/>
+      </c>
+      <c r="E72" s="42" t="str">
+        <v>A, B, C</v>
+      </c>
+      <c r="F72" s="44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="42"/>
+      <c r="F73" s="44"/>
+    </row>
+    <row r="74" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B74" s="43"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="42"/>
+      <c r="F74" s="44"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>

</xml_diff>